<commit_message>
Code Check In 13 Oct
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/bin/com/mojio/xls/ImportSIMs.xlsx
+++ b/MyMojioWebsite/bin/com/mojio/xls/ImportSIMs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -291,7 +291,7 @@
     <t>Click on Upload Checkbox</t>
   </si>
   <si>
-    <t>simUploadnableXpath</t>
+    <t>simUploadEnableXpath</t>
   </si>
   <si>
     <t>Verify the Browse Field is Enabled</t>
@@ -300,12 +300,6 @@
     <t>verifyElementEnabledId</t>
   </si>
   <si>
-    <t>Verify the CSV format import  is disabled</t>
-  </si>
-  <si>
-    <t>Verify the APN field is disabled</t>
-  </si>
-  <si>
     <t>Verify the No file Upload Error</t>
   </si>
   <si>
@@ -372,7 +366,7 @@
     <t>CSV_Format_Error</t>
   </si>
   <si>
-    <t>This field is required. </t>
+    <t>This field is required</t>
   </si>
   <si>
     <t>File_Browse_Error</t>
@@ -494,7 +488,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -552,10 +546,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -639,7 +629,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+      <selection activeCell="C8" activeCellId="0" pane="topLeft" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -770,17 +760,17 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
@@ -805,7 +795,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -816,23 +806,23 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -854,10 +844,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:77"/>
+  <dimension ref="1:75"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A46" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A67" activeCellId="0" pane="topLeft" sqref="A67"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E66" activeCellId="0" pane="topLeft" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1122,6 +1112,8 @@
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="AMC11" s="0"/>
+      <c r="AMD11" s="0"/>
       <c r="AME11" s="0"/>
       <c r="AMF11" s="0"/>
       <c r="AMG11" s="0"/>
@@ -1150,6 +1142,8 @@
       <c r="H12" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="AMC12" s="0"/>
+      <c r="AMD12" s="0"/>
       <c r="AME12" s="0"/>
       <c r="AMF12" s="0"/>
       <c r="AMG12" s="0"/>
@@ -1178,6 +1172,8 @@
       <c r="H13" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="AMC13" s="0"/>
+      <c r="AMD13" s="0"/>
       <c r="AME13" s="0"/>
       <c r="AMF13" s="0"/>
       <c r="AMG13" s="0"/>
@@ -1623,6 +1619,9 @@
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
+      <c r="H33" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="5" t="s">
@@ -1640,6 +1639,9 @@
       <c r="E34" s="5"/>
       <c r="F34" s="12"/>
       <c r="G34" s="5"/>
+      <c r="H34" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="5" t="s">
@@ -1657,6 +1659,9 @@
       <c r="E35" s="5"/>
       <c r="F35" s="12"/>
       <c r="G35" s="5"/>
+      <c r="H35" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="5" t="s">
@@ -1676,6 +1681,9 @@
         <v>78</v>
       </c>
       <c r="G36" s="5"/>
+      <c r="H36" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="5" t="s">
@@ -1695,6 +1703,9 @@
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
+      <c r="H37" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="7" t="s">
@@ -1714,6 +1725,9 @@
         <v>27</v>
       </c>
       <c r="G38" s="7"/>
+      <c r="H38" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="7" t="s">
@@ -1733,6 +1747,9 @@
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
+      <c r="H39" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="7" t="s">
@@ -1752,6 +1769,9 @@
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
+      <c r="H40" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="7" t="s">
@@ -1771,6 +1791,9 @@
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
+      <c r="H41" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="7" t="s">
@@ -1790,6 +1813,9 @@
         <v>59</v>
       </c>
       <c r="G42" s="7"/>
+      <c r="H42" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="7" t="s">
@@ -1811,6 +1837,9 @@
         <v>66</v>
       </c>
       <c r="G43" s="7"/>
+      <c r="H43" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="7" t="s">
@@ -1830,6 +1859,9 @@
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
+      <c r="H44" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="7" t="s">
@@ -1849,6 +1881,9 @@
         <v>83</v>
       </c>
       <c r="G45" s="7"/>
+      <c r="H45" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="9" t="s">
@@ -1868,6 +1903,9 @@
         <v>27</v>
       </c>
       <c r="G46" s="9"/>
+      <c r="H46" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="9" t="s">
@@ -1887,6 +1925,9 @@
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
+      <c r="H47" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="9" t="s">
@@ -1906,6 +1947,9 @@
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
+      <c r="H48" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="9" t="s">
@@ -1925,6 +1969,9 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
+      <c r="H49" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="9" t="s">
@@ -1944,6 +1991,9 @@
         <v>59</v>
       </c>
       <c r="G50" s="9"/>
+      <c r="H50" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="9" t="s">
@@ -1963,6 +2013,9 @@
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
+      <c r="H51" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="9" t="s">
@@ -1982,6 +2035,9 @@
         <v>83</v>
       </c>
       <c r="G52" s="9"/>
+      <c r="H52" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="5" t="s">
@@ -2001,6 +2057,9 @@
         <v>27</v>
       </c>
       <c r="G53" s="5"/>
+      <c r="H53" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="5" t="s">
@@ -2020,6 +2079,9 @@
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
+      <c r="H54" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="5" t="s">
@@ -2039,6 +2101,9 @@
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
+      <c r="H55" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="5" t="s">
@@ -2058,6 +2123,9 @@
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
+      <c r="H56" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="5" t="s">
@@ -2077,6 +2145,9 @@
         <v>59</v>
       </c>
       <c r="G57" s="5"/>
+      <c r="H57" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="5" t="s">
@@ -2096,6 +2167,9 @@
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
+      <c r="H58" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="59">
       <c r="A59" s="7" t="s">
@@ -2115,6 +2189,9 @@
         <v>27</v>
       </c>
       <c r="G59" s="7"/>
+      <c r="H59" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="7" t="s">
@@ -2134,6 +2211,9 @@
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
+      <c r="H60" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="7" t="s">
@@ -2153,6 +2233,9 @@
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
+      <c r="H61" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="7" t="s">
@@ -2172,6 +2255,9 @@
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
+      <c r="H62" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="7" t="s">
@@ -2191,6 +2277,9 @@
         <v>59</v>
       </c>
       <c r="G63" s="7"/>
+      <c r="H63" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="7" t="s">
@@ -2210,6 +2299,9 @@
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
+      <c r="H64" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="7" t="s">
@@ -2229,242 +2321,227 @@
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
+      <c r="H65" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="66">
-      <c r="A66" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
+      <c r="A66" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G66" s="10"/>
+      <c r="H66" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="67">
-      <c r="A67" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
+      <c r="A67" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F67" s="9"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F68" s="9"/>
       <c r="G68" s="10"/>
+      <c r="H68" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="10"/>
+      <c r="H69" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F70" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="G70" s="10"/>
+      <c r="H70" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="10"/>
+      <c r="H71" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9" t="s">
-        <v>59</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F72" s="9"/>
       <c r="G72" s="10"/>
+      <c r="H72" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="10"/>
+      <c r="H73" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F74" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="G74" s="10"/>
+      <c r="H74" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
-      <c r="A76" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G76" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
-      <c r="A77" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
-      <c r="P77" s="15"/>
-      <c r="Q77" s="15"/>
-      <c r="R77" s="15"/>
-      <c r="S77" s="15"/>
+      <c r="H75" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2500,16 +2577,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
@@ -2517,16 +2594,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
@@ -2563,7 +2640,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
@@ -2571,7 +2648,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
@@ -2611,16 +2688,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>109</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
@@ -2628,16 +2705,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
@@ -2673,29 +2750,29 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>4</v>
@@ -2720,7 +2797,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2731,29 +2808,29 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>4</v>
@@ -2778,7 +2855,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2788,23 +2865,23 @@
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -2840,7 +2917,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
@@ -2848,7 +2925,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>

</xml_diff>